<commit_message>
Cleaned and set all networks to run from .mat flies
</commit_message>
<xml_diff>
--- a/MLP_with_PSO/NN_output data/_fitness_results_complex_cosine.xlsx
+++ b/MLP_with_PSO/NN_output data/_fitness_results_complex_cosine.xlsx
@@ -441,252 +441,252 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.466847241961997</v>
+        <v>0.8838797317479079</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.2662009302792725</v>
+        <v>0.5804756250896509</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.153346737789284</v>
+        <v>0.5689877857268043</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.153346737789284</v>
+        <v>0.5560926013731577</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.2248840404696891</v>
+        <v>0.6009613394303588</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.5641950586202509</v>
+        <v>0.7116331327055651</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.4147354104590233</v>
+        <v>0.678844926177689</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.4028443483674213</v>
+        <v>0.4874762401984203</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.3303669052154103</v>
+        <v>0.4454385935230377</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.2738901935240512</v>
+        <v>0.3114347509580857</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.2262149153965591</v>
+        <v>0.3349623807193612</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.1973375083707292</v>
+        <v>0.1746741661377086</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.1672521289339457</v>
+        <v>0.2179316971256372</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.1372805991341141</v>
+        <v>0.1859517758672763</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.1351733821481619</v>
+        <v>0.1581025253002655</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.1199692097252694</v>
+        <v>0.1287986758911418</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.1110539756474304</v>
+        <v>0.1072357221515841</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.1000126926264591</v>
+        <v>0.09948603012936319</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.1023750525218791</v>
+        <v>0.09377771078667768</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.1009915612131791</v>
+        <v>0.093224478992346</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.1004821003091073</v>
+        <v>0.08882978148549628</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.09863705979159483</v>
+        <v>0.08858154975821175</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.09560328677546252</v>
+        <v>0.08909639842212708</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.09268252163453669</v>
+        <v>0.08806155458954379</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.09045124430112184</v>
+        <v>0.0856825622416382</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.08996810295694704</v>
+        <v>0.08596083630439189</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.08956520937765981</v>
+        <v>0.08520685196275338</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.08907902059384985</v>
+        <v>0.08515360638446175</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.08888438907463149</v>
+        <v>0.08510105188471401</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.0888078287238319</v>
+        <v>0.0849349134539981</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.08860779741088361</v>
+        <v>0.08492314055169457</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.08849570079299568</v>
+        <v>0.08484652061346608</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.08844859927161103</v>
+        <v>0.0848629246688912</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.08831222861866574</v>
+        <v>0.08483236540724776</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.08825342881541237</v>
+        <v>0.08477981081747249</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.08823663759260672</v>
+        <v>0.08475837594653182</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.08822702520875265</v>
+        <v>0.08475730470400228</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.08821071226192778</v>
+        <v>0.08474557933377681</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.0881834262680114</v>
+        <v>0.08471829387392681</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.08817876634941803</v>
+        <v>0.08474114510300992</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.08817102958001781</v>
+        <v>0.08476343409439994</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.08816193175737362</v>
+        <v>0.08472204855566307</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.08816438707840246</v>
+        <v>0.08466100834992524</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.08816587155191601</v>
+        <v>0.08464032251196726</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.08816756726076468</v>
+        <v>0.08460949939466041</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.08816564793073789</v>
+        <v>0.08458676911291615</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.0881600057199953</v>
+        <v>0.08456284622344548</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.08815545409985331</v>
+        <v>0.08454967045776435</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.08814997530408186</v>
+        <v>0.08453807217629299</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0.08814793386216974</v>
+        <v>0.0845354999738257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>